<commit_message>
CHS-Allgather results are added
</commit_message>
<xml_diff>
--- a/MVAPICH/Results/NoleLand/NewSystem/SecureAlltoall/NS-AlltoAll-MVAPICH.xlsx
+++ b/MVAPICH/Results/NoleLand/NewSystem/SecureAlltoall/NS-AlltoAll-MVAPICH.xlsx
@@ -135,7 +135,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -157,7 +156,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -165,14 +163,12 @@
       <color rgb="FF000000"/>
       <name val="Raleway"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Raleway"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -180,7 +176,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -332,6 +327,8 @@
   <dxfs count="1">
     <dxf>
       <font>
+        <name val="Arial"/>
+        <family val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -411,13 +408,13 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H63" activeCellId="0" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="1" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -3833,13 +3830,13 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H63" activeCellId="0" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="1" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -7255,13 +7252,13 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H63" activeCellId="0" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="1" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -10677,13 +10674,13 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H63" activeCellId="0" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="1" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -14099,13 +14096,13 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H63" activeCellId="0" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="1" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -17521,16 +17518,16 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G61" activeCellId="0" sqref="G61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1003" min="3" style="1" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1004" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="3" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1004" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21007,14 +21004,9 @@
       <formula>B5=MIN($B5:$F5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61:F82">
+  <conditionalFormatting sqref="B61:F82 B89:F110">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>B61=MIN($B61:$F61)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B89:F110">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>B89=MIN($B89:$F89)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>